<commit_message>
Upload for hyipworld flow
</commit_message>
<xml_diff>
--- a/images/github/doc/infoworld.xlsx
+++ b/images/github/doc/infoworld.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="info-world" sheetId="1" r:id="rId1"/>
+    <sheet name="monitor-rating" sheetId="4" r:id="rId2"/>
+    <sheet name="script-team" sheetId="5" r:id="rId3"/>
+    <sheet name="hyip-world" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="9">
   <si>
     <t>repo</t>
   </si>
@@ -32,12 +33,24 @@
   <si>
     <t>world</t>
   </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -288,11 +301,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -321,12 +354,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -405,6 +448,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -439,6 +483,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -614,16 +659,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
@@ -634,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
         <v>0</v>
@@ -646,7 +691,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="4"/>
       <c r="C4" s="8"/>
@@ -656,7 +701,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="21" t="s">
@@ -670,7 +715,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="22"/>
@@ -679,24 +724,27 @@
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="12"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="C8" s="20" t="str">
+        <f>G2</f>
+        <v>world</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>F2</f>
+        <v>hyip</v>
+      </c>
+      <c r="G8" t="str">
+        <f>C2</f>
+        <v>info</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="25"/>
       <c r="C9" s="7" t="s">
@@ -709,7 +757,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="8"/>
@@ -719,7 +767,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="7" t="s">
@@ -733,7 +781,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="8"/>
       <c r="D12" s="2"/>
@@ -741,23 +789,26 @@
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="C14" s="20" t="str">
+        <f>C2</f>
+        <v>info</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>F8</f>
+        <v>hyip</v>
+      </c>
+      <c r="G14" t="str">
+        <f>G2</f>
+        <v>world</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="5"/>
       <c r="C15" s="16" t="s">
@@ -770,7 +821,7 @@
       </c>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="17"/>
@@ -780,7 +831,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
       <c r="C17" s="23" t="s">
@@ -794,7 +845,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="24"/>
       <c r="D18" s="10"/>
@@ -809,25 +860,858 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="20" t="str">
+        <f>G2</f>
+        <v>rating</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>F2</f>
+        <v>hyip</v>
+      </c>
+      <c r="G8" t="str">
+        <f>C2</f>
+        <v>monitor</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="20" t="str">
+        <f>C2</f>
+        <v>monitor</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>F8</f>
+        <v>hyip</v>
+      </c>
+      <c r="G14" t="str">
+        <f>G2</f>
+        <v>rating</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="19"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="20" t="str">
+        <f>G2</f>
+        <v>team</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>F2</f>
+        <v>hyip</v>
+      </c>
+      <c r="G8" t="str">
+        <f>C2</f>
+        <v>script</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="20" t="str">
+        <f>C2</f>
+        <v>script</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>F8</f>
+        <v>hyip</v>
+      </c>
+      <c r="G14" t="str">
+        <f>G2</f>
+        <v>team</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="19"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="18"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="18"/>
+      <c r="H41" s="17"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="15"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>